<commit_message>
SQL Insert change, log failed move file activity
</commit_message>
<xml_diff>
--- a/Data/OutputTableRows.xlsx
+++ b/Data/OutputTableRows.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\libor\Dropbox\LK_docs\Valuetools\Zákazníci\Benet Automotive\Demo Process\Invoice-RossumDataExport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF18088F-9CF0-40A2-B616-E1F0962E69B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E91670-656B-4D9F-8788-1E72C0DACAB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Variabilní symbol</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>ID_Import_SAP</t>
+  </si>
+  <si>
+    <t>Číslo faktury</t>
+  </si>
+  <si>
+    <t>Invoice Number</t>
+  </si>
+  <si>
+    <t>Invoice_number</t>
   </si>
 </sst>
 </file>
@@ -530,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,115 +612,126 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>